<commit_message>
Changed rank of omni talent from 10 to 9. Add "scroll" to all related card name. Changed all robot card effects to avoid rank change at hand.
</commit_message>
<xml_diff>
--- a/sheet/ItemCardData.xlsx
+++ b/sheet/ItemCardData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A8CC3D-A09E-4D6D-A9AB-E7DED5E1DB5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C4698B-8495-4B55-8CDE-836D3002F726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6285" yWindow="4140" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="164">
   <si>
     <t>蔬菜罐头</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -181,10 +181,6 @@
     <t>Can be used when Player wins in a battle round with more total rank: Cost 1 scroll Then add a card of your side to your hand instead of discarding it. This effect can be used multiple times for every battle round.</t>
   </si>
   <si>
-    <t>灭绝</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Genocide</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -193,10 +189,6 @@
 Can be used before making actions: Cost X scroll. Then select { monster } cards with a total rank of X from Exploration Zone and send them to Graveyard.</t>
   </si>
   <si>
-    <t>点金</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Midas touch</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -205,19 +197,11 @@
 Can be used before making actions: Cost 1 scroll. Then select a { Monster } card with a rank no more than three from your hand. Send that card to Graveyard and get X unity of gold. X is the rank of that card.</t>
   </si>
   <si>
-    <t>变化</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Polymorph</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Can be used before making actions: Cost 1 scroll. Then redraw a { monster } card in Exploration Zone.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>援军</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -234,18 +218,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>解除陷阱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Can be used before making actions: Cost 1 scroll. Then send a { Trap } card in Exploration Zone to Graveyard.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>祝福</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Bless</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -253,18 +229,10 @@
     <t>Can be used before a battle round: Cost 1 scroll. Increase the rank of a card of your side by one.</t>
   </si>
   <si>
-    <t>诅咒</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Curse</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>传送他人</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Teleport others</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -272,10 +240,6 @@
     <t>Can be used before making actions: Cost 1 scroll. Then shuffle a { Monster } card in Exploration Zone to Main Deck.</t>
   </si>
   <si>
-    <t>长距离传送</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Teleport</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -334,10 +298,6 @@
   </si>
   <si>
     <t>Can be used before making actions: Cost 1 ammo. Then select two cards from your hand or Exploration Zone and swap them.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>金币枪</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -393,14 +353,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>结界</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lich Sword</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>预见针剂</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -542,18 +494,6 @@
   </si>
   <si>
     <t>选手牌1张怪物牌弃置，将房间区所有含有那张牌标签的怪物牌送墓。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>融合</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>选房间区和手牌各1张怪物牌，从主牌堆选1张点数与这两张牌的合计点数相同、且标签与这两张牌均没有交集的怪物牌，加入手牌或放到房间区任意列最前方。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>驱散</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -686,6 +626,62 @@
   </si>
   <si>
     <t>Oil lamp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选房间区和手牌各1张怪物牌，从主牌堆选1张点数与这两张牌的合计点数相同的怪物牌，加入手牌或放到房间区任意列最前方。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>融合卷轴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>驱散卷轴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>灭绝卷轴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点金卷轴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>变化卷轴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>援军卷轴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>解除陷阱卷轴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>祝福卷轴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>诅咒卷轴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>传送他人卷轴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>传送卷轴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>结界卷轴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>硬币枪</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1030,73 +1026,71 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E1" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="114" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>162</v>
       </c>
       <c r="B2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>92</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="3" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="114" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="171" x14ac:dyDescent="0.2">
@@ -1107,7 +1101,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>1</v>
@@ -1124,7 +1118,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>4</v>
@@ -1141,7 +1135,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>7</v>
@@ -1158,7 +1152,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -1175,7 +1169,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>13</v>
@@ -1192,7 +1186,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>16</v>
@@ -1209,7 +1203,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>19</v>
@@ -1226,7 +1220,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>22</v>
@@ -1243,7 +1237,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>25</v>
@@ -1254,13 +1248,13 @@
     </row>
     <row r="14" spans="1:6" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>27</v>
@@ -1277,7 +1271,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>30</v>
@@ -1288,13 +1282,13 @@
     </row>
     <row r="16" spans="1:6" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B16" s="1">
         <v>2</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>32</v>
@@ -1311,7 +1305,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>35</v>
@@ -1320,444 +1314,444 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="256.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="B18" s="1">
         <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="B19" s="1">
         <v>2</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" ht="370.5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>153</v>
       </c>
       <c r="B20" s="1">
         <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>154</v>
       </c>
       <c r="B21" s="1">
         <v>3</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>155</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>156</v>
       </c>
       <c r="B23" s="1">
         <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B24" s="1">
         <v>3</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>157</v>
       </c>
       <c r="B25" s="1">
         <v>2</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="B26" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>159</v>
       </c>
       <c r="B27" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="B28" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="270.75" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>161</v>
       </c>
       <c r="B29" s="1">
         <v>2</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B30" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="299.25" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B31" s="1">
         <v>1</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B32" s="1">
         <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="313.5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B33" s="1">
         <v>2</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="228" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B34" s="1">
         <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="327.75" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>163</v>
       </c>
       <c r="B35" s="1">
         <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="299.25" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="B36">
         <v>3</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="299.25" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="114" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="B38">
         <v>3</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="E38" s="3"/>
     </row>
     <row r="39" spans="1:5" ht="327.75" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="B39">
         <v>2</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="342" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="270.75" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="B41">
         <v>2</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="270.75" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="B42">
         <v>2</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="228" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="B44">
         <v>2</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed rank of Teleport Other from 1 to 2. Changed rank of Miner Bot from 2 to 1. Changed rank of Mini Factory from 1 to 2.
</commit_message>
<xml_diff>
--- a/sheet/ItemCardData.xlsx
+++ b/sheet/ItemCardData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030B0792-E086-47BC-8C17-E55FD991B5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958671C2-FCB4-46E2-B8A9-3A27BA19E93D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1815" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1020,7 +1020,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1492,7 +1492,7 @@
         <v>122</v>
       </c>
       <c r="C25" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
Change cost of Teleport Other from 1 to 2. Add a scroll item card Jet Lag. Changed the effect of Disguise, making it much stronger. Changed the effect of Mini Factory and Watchdog Bot.
</commit_message>
<xml_diff>
--- a/sheet/ItemCardData.xlsx
+++ b/sheet/ItemCardData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958671C2-FCB4-46E2-B8A9-3A27BA19E93D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCD110A-9CA8-472F-846A-450FAB3F0276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1815" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="165">
   <si>
     <t>蔬菜罐头</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -675,6 +675,14 @@
   </si>
   <si>
     <t>宣言1个种族，消灭手牌和场上所有那个种族的怪物牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间跳跃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>牌通过移动后可以发动：将那张牌复位。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1017,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1370,65 +1378,65 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
       <c r="B19" t="s">
         <v>108</v>
       </c>
       <c r="C19" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="185.25" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B20" t="s">
         <v>108</v>
       </c>
       <c r="C20" s="1">
+        <v>4</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="185.25" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>126</v>
+      </c>
+      <c r="B21" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="1">
         <v>1</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="57" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="22" spans="1:6" ht="57" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>127</v>
-      </c>
-      <c r="B21" t="s">
-        <v>122</v>
-      </c>
-      <c r="C21" s="1">
-        <v>2</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" ht="199.5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>132</v>
       </c>
       <c r="B22" t="s">
         <v>122</v>
@@ -1437,38 +1445,34 @@
         <v>2</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="185.25" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B23" t="s">
         <v>122</v>
       </c>
       <c r="C23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="85.5" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B24" t="s">
         <v>122</v>
@@ -1477,36 +1481,36 @@
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" ht="213.75" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B25" t="s">
         <v>122</v>
       </c>
       <c r="C25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>75</v>
+        <v>148</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="270.75" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B26" t="s">
         <v>122</v>
@@ -1515,74 +1519,74 @@
         <v>2</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="270.75" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>136</v>
+      </c>
+      <c r="B27" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F27" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="128.25" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="28" spans="1:6" ht="128.25" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>156</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>108</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C28" s="1">
         <v>1</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:6" ht="57" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" ht="57" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>104</v>
-      </c>
-      <c r="B28" t="s">
-        <v>137</v>
-      </c>
-      <c r="C28" s="1">
-        <v>2</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" ht="299.25" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>140</v>
       </c>
       <c r="B29" t="s">
         <v>137</v>
       </c>
       <c r="C29" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>138</v>
+        <v>105</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="185.25" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" ht="299.25" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>140</v>
       </c>
       <c r="B30" t="s">
         <v>137</v>
@@ -1591,38 +1595,38 @@
         <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>50</v>
+        <v>106</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="228" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
         <v>137</v>
       </c>
       <c r="C31" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="327.75" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="228" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
         <v>137</v>
@@ -1631,204 +1635,224 @@
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="327.75" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" t="s">
+        <v>137</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F33" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="299.25" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="34" spans="1:6" ht="299.25" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>77</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <v>3</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F34" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="142.5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="35" spans="1:6" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>159</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C35" s="1">
         <v>1</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" ht="299.25" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="E35" s="2"/>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="1:6" ht="299.25" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>81</v>
       </c>
-      <c r="C35">
-        <v>2</v>
-      </c>
-      <c r="D35" s="1" t="s">
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F36" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="57" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="37" spans="1:6" ht="57" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>84</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <v>0</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="1:6" ht="327.75" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:6" ht="327.75" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>85</v>
       </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="D37" s="1" t="s">
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="342" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="39" spans="1:6" ht="342" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>87</v>
       </c>
-      <c r="C38">
+      <c r="C39">
         <v>1</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F39" s="3" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="270.75" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>91</v>
-      </c>
-      <c r="C39">
-        <v>2</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="270.75" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="270.75" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>94</v>
       </c>
-      <c r="C40">
-        <v>2</v>
-      </c>
-      <c r="D40" s="1" t="s">
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F41" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="228" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="42" spans="1:6" ht="228" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>97</v>
       </c>
-      <c r="C41">
+      <c r="C42">
         <v>1</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F42" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="43" spans="1:6" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>64</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C43" s="1">
         <v>3</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F43" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="213.75" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="44" spans="1:6" ht="213.75" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>72</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C44" s="1">
         <v>1</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F44" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="45" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>152</v>
       </c>
-      <c r="C44">
+      <c r="C45">
         <v>1</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>153</v>
       </c>
     </row>

</xml_diff>